<commit_message>
commiting C42203 testcse scripts
</commit_message>
<xml_diff>
--- a/Testdata/Non_Oncology/BaseFile.xlsx
+++ b/Testdata/Non_Oncology/BaseFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\Non_Oncology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PSE WORKSPACE\pse.autotest\Testdata\Non_Oncology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2BD984-537B-4CF1-BADD-A623B904106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319278E6-86C8-4609-91A9-0886EE25BE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Environment</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t>nononco_geographic_section_clientuser_validation</t>
+  </si>
+  <si>
+    <t>livehta_3750_manage_abbreviation</t>
+  </si>
+  <si>
+    <t>\Testdata\Non_Oncology\DataFiles\ManageAbbreviations\LIVEHTA_3750_manageAbbreviation_Data.xlsx</t>
   </si>
 </sst>
 </file>
@@ -508,22 +514,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -545,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -556,7 +562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -567,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -578,7 +584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -589,7 +595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -600,7 +606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -611,7 +617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -622,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -633,7 +639,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -644,7 +650,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -655,7 +661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -666,7 +672,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -677,7 +683,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -688,7 +694,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -699,7 +705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -710,7 +716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -721,7 +727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -732,7 +738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -743,7 +749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -754,7 +760,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -765,7 +771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -776,7 +782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -787,7 +793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -796,6 +802,17 @@
       </c>
       <c r="C25" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>